<commit_message>
Update Kenya source XLSX
</commit_message>
<xml_diff>
--- a/data/xlsx/KE.xlsx
+++ b/data/xlsx/KE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB199FE8-4847-2540-9EEB-0C4F48828BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099C6461-04D0-E04F-AC8E-ED6AB37F4F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38780" yWindow="-1080" windowWidth="26040" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45320" yWindow="-1080" windowWidth="19500" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KE" sheetId="1" r:id="rId1"/>
@@ -1979,7 +1979,7 @@
   <dimension ref="A1:B127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3013,7 +3013,7 @@
   <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>